<commit_message>
version 19/06:code complet et code fitting
</commit_message>
<xml_diff>
--- a/Data Komilis FWGW.xlsx
+++ b/Data Komilis FWGW.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hravoaha\Desktop\Thèse\composting code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AEA0E9-471F-4F4F-BA04-A7B6A91C9922}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD54FE8-57C8-4AA0-BE23-673E892880A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="6" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Composition of waste" sheetId="4" r:id="rId1"/>
     <sheet name="Composition (mass)" sheetId="6" r:id="rId2"/>
     <sheet name="Variables" sheetId="1" r:id="rId3"/>
-    <sheet name="stoe" sheetId="7" r:id="rId4"/>
-    <sheet name="Xyield" sheetId="10" r:id="rId5"/>
+    <sheet name="Xyield" sheetId="10" r:id="rId4"/>
+    <sheet name="stoe" sheetId="7" r:id="rId5"/>
     <sheet name="kinetics" sheetId="2" r:id="rId6"/>
     <sheet name="tech" sheetId="3" r:id="rId7"/>
     <sheet name="aer" sheetId="9" r:id="rId8"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="652">
   <si>
     <t>Valeurs</t>
   </si>
@@ -1989,6 +1989,12 @@
   </si>
   <si>
     <t>m(N-org)(g)</t>
+  </si>
+  <si>
+    <t>Y(X/O2)(molX/molO2)</t>
+  </si>
+  <si>
+    <t>Y (kgX/kgS)</t>
   </si>
 </sst>
 </file>
@@ -2661,7 +2667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A43F10C-4AB5-4A1F-A346-6667884FAA0F}">
   <dimension ref="A1:CE113"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A96" sqref="A96:XFD96"/>
     </sheetView>
@@ -25966,7 +25972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DF1B96-6F36-403A-A03F-B41BA123E54D}">
   <dimension ref="A1:CD106"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
@@ -50456,8 +50462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13E0657-BE6C-45BC-B891-D54361BD0D37}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51673,11 +51679,969 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD039EB6-CAC1-4780-9B81-62B23D513731}">
+  <dimension ref="A1:AL28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D1" t="s">
+        <v>607</v>
+      </c>
+      <c r="E1" t="s">
+        <v>608</v>
+      </c>
+      <c r="F1" t="s">
+        <v>609</v>
+      </c>
+      <c r="G1" t="s">
+        <v>637</v>
+      </c>
+      <c r="H1" t="s">
+        <v>619</v>
+      </c>
+      <c r="L1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B2">
+        <v>0.35</v>
+      </c>
+      <c r="C2">
+        <f>(Variables!L14/Variables!L23)*(stoe!B3/(6-(5*stoe!B3)))</f>
+        <v>0.61286157024793375</v>
+      </c>
+      <c r="D2">
+        <f>(Variables!M14/Variables!L26)</f>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="E2">
+        <f>(stoe!B3/(6-5*(stoe!B3)))*(Variables!L14/Variables!L24)</f>
+        <v>0.44571750563486096</v>
+      </c>
+      <c r="F2">
+        <f>(Variables!L14/Variables!L22)*(stoe!B3/(6-(2*stoe!B3)))</f>
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="H2" t="s">
+        <v>620</v>
+      </c>
+      <c r="J2">
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="L2">
+        <f>C2*(Variables!L$23/Variables!L$14)</f>
+        <v>0.17355371900826441</v>
+      </c>
+      <c r="O2">
+        <v>0.17355371900826441</v>
+      </c>
+      <c r="P2">
+        <v>9.8678414096916287E-2</v>
+      </c>
+      <c r="Q2">
+        <v>4.4403195867968683E-2</v>
+      </c>
+      <c r="R2">
+        <v>0.17355371900826441</v>
+      </c>
+      <c r="S2">
+        <v>9.8678414096916287E-2</v>
+      </c>
+      <c r="T2">
+        <v>4.4403195867968683E-2</v>
+      </c>
+      <c r="U2">
+        <v>0.17355371900826441</v>
+      </c>
+      <c r="V2">
+        <v>9.8678414096916287E-2</v>
+      </c>
+      <c r="W2">
+        <v>4.4403195867968683E-2</v>
+      </c>
+      <c r="X2">
+        <v>5.4361283061339333E-2</v>
+      </c>
+      <c r="Y2">
+        <v>0.17355371900826441</v>
+      </c>
+      <c r="Z2">
+        <v>9.8678414096916287E-2</v>
+      </c>
+      <c r="AA2">
+        <v>4.4403195867968683E-2</v>
+      </c>
+      <c r="AB2">
+        <v>5.4361283061339333E-2</v>
+      </c>
+      <c r="AC2">
+        <v>7.6782449725776941E-2</v>
+      </c>
+      <c r="AD2">
+        <v>4.4286279161724E-2</v>
+      </c>
+      <c r="AE2">
+        <v>1.9267471870961863E-2</v>
+      </c>
+      <c r="AF2">
+        <v>2.4607076444965226E-2</v>
+      </c>
+      <c r="AG2">
+        <v>2.7217966832750799E-2</v>
+      </c>
+      <c r="AH2">
+        <v>7.6782449725776941E-2</v>
+      </c>
+      <c r="AI2">
+        <v>4.4286279161724E-2</v>
+      </c>
+      <c r="AJ2">
+        <v>1.9267471870961863E-2</v>
+      </c>
+      <c r="AK2">
+        <v>2.4607076444965226E-2</v>
+      </c>
+      <c r="AL2">
+        <v>2.7217966832750799E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>582</v>
+      </c>
+      <c r="B3">
+        <v>0.35</v>
+      </c>
+      <c r="C3">
+        <f>(Variables!L15/Variables!L23)*(stoe!B4/((33/2)-(5*stoe!B4)))</f>
+        <v>0.34845814977973566</v>
+      </c>
+      <c r="D3">
+        <f>(Variables!L14/Variables!L26)*(stoe!B4/(4-stoe!B4))</f>
+        <v>2.4906254472591955</v>
+      </c>
+      <c r="E3">
+        <f>(Variables!L14/Variables!L24)*(stoe!B4/(15-(5*stoe!B4)))</f>
+        <v>0.29323447636700645</v>
+      </c>
+      <c r="F3">
+        <f>(Variables!L14/Variables!L22)*(stoe!B4/(6-(2*stoe!B4)))</f>
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="H3" t="s">
+        <v>621</v>
+      </c>
+      <c r="J3">
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="L3">
+        <f>C3*(Variables!L$23/Variables!L$14)</f>
+        <v>9.8678414096916287E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B4">
+        <v>0.35</v>
+      </c>
+      <c r="C4">
+        <f>(Variables!L14/Variables!L23)*(stoe!B5/((134/4)-(5*stoe!B5)))</f>
+        <v>0.15679878540876441</v>
+      </c>
+      <c r="D4">
+        <f>(Variables!L14/Variables!L26)</f>
+        <v>6.6470588235294121</v>
+      </c>
+      <c r="E4">
+        <f>(Variables!L14/Variables!L24)*(stoe!B5/(25-(5*stoe!B5)))</f>
+        <v>0.16528408426291219</v>
+      </c>
+      <c r="F4">
+        <f>(Variables!L14/Variables!L22)*(stoe!B5/((45/2)-(2*stoe!B5)))</f>
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="H4" t="s">
+        <v>622</v>
+      </c>
+      <c r="J4">
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="L4">
+        <f>C4*(Variables!L$23/Variables!L$14)</f>
+        <v>4.4403195867968683E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>584</v>
+      </c>
+      <c r="B5">
+        <v>0.35</v>
+      </c>
+      <c r="C5">
+        <f>C2</f>
+        <v>0.61286157024793375</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:F5" si="0">D2</f>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.44571750563486096</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="H5" t="s">
+        <v>623</v>
+      </c>
+      <c r="J5">
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="L5">
+        <f>C5*(Variables!L$23/Variables!L$14)</f>
+        <v>0.17355371900826441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>585</v>
+      </c>
+      <c r="B6">
+        <v>0.35</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:F6" si="1">C3</f>
+        <v>0.34845814977973566</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.4906254472591955</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.29323447636700645</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="H6" t="s">
+        <v>624</v>
+      </c>
+      <c r="J6">
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="L6">
+        <f>C6*(Variables!L$23/Variables!L$14)</f>
+        <v>9.8678414096916287E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>586</v>
+      </c>
+      <c r="B7">
+        <v>0.35</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:F7" si="2">C4</f>
+        <v>0.15679878540876441</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>6.6470588235294121</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.16528408426291219</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="H7" t="s">
+        <v>625</v>
+      </c>
+      <c r="J7">
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="L7">
+        <f>C7*(Variables!L$23/Variables!L$14)</f>
+        <v>4.4403195867968683E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>587</v>
+      </c>
+      <c r="B8">
+        <v>0.35</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="3">C2</f>
+        <v>0.61286157024793375</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>0.44571750563486096</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="H8" t="s">
+        <v>626</v>
+      </c>
+      <c r="J8">
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="L8">
+        <f>C8*(Variables!L$23/Variables!L$14)</f>
+        <v>0.17355371900826441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>588</v>
+      </c>
+      <c r="B9">
+        <v>0.35</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:F9" si="4">C3</f>
+        <v>0.34845814977973566</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="4"/>
+        <v>2.4906254472591955</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>0.29323447636700645</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="H9" t="s">
+        <v>627</v>
+      </c>
+      <c r="J9">
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="L9">
+        <f>C9*(Variables!L$23/Variables!L$14)</f>
+        <v>9.8678414096916287E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>589</v>
+      </c>
+      <c r="B10">
+        <v>0.35</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:F10" si="5">C4</f>
+        <v>0.15679878540876441</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="5"/>
+        <v>6.6470588235294121</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="5"/>
+        <v>0.16528408426291219</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="5"/>
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="H10" t="s">
+        <v>628</v>
+      </c>
+      <c r="J10">
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="L10">
+        <f>C10*(Variables!L$23/Variables!L$14)</f>
+        <v>4.4403195867968683E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>590</v>
+      </c>
+      <c r="B11">
+        <v>0.35</v>
+      </c>
+      <c r="C11">
+        <f>(Variables!L16/Variables!L23)*(stoe!B6/(10-(5*stoe!B6)))</f>
+        <v>0.19196328081035452</v>
+      </c>
+      <c r="D11">
+        <f>(Variables!L16/Variables!L26)</f>
+        <v>6.6470588235294121</v>
+      </c>
+      <c r="E11">
+        <f>(Variables!L16/Variables!L24)*(stoe!B6/(10-(5*stoe!B6)))</f>
+        <v>0.13960965877116693</v>
+      </c>
+      <c r="F11">
+        <f>(Variables!L16/Variables!L22)*(stoe!B6/(9-(2*stoe!B6)))</f>
+        <v>0.32944009850789513</v>
+      </c>
+      <c r="H11" t="s">
+        <v>629</v>
+      </c>
+      <c r="J11">
+        <v>0.32944009850789513</v>
+      </c>
+      <c r="L11">
+        <f>C11*(Variables!L$23/Variables!L$14)</f>
+        <v>5.4361283061339333E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>591</v>
+      </c>
+      <c r="B12">
+        <v>0.35</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:F12" si="6">C2</f>
+        <v>0.61286157024793375</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="6"/>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="6"/>
+        <v>0.44571750563486096</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="6"/>
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="H12" t="s">
+        <v>630</v>
+      </c>
+      <c r="J12">
+        <v>0.71648550724637672</v>
+      </c>
+      <c r="L12">
+        <f>C12*(Variables!L$23/Variables!L$14)</f>
+        <v>0.17355371900826441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>592</v>
+      </c>
+      <c r="B13">
+        <v>0.35</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:F13" si="7">C3</f>
+        <v>0.34845814977973566</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="7"/>
+        <v>2.4906254472591955</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="7"/>
+        <v>0.29323447636700645</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="7"/>
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="H13" t="s">
+        <v>631</v>
+      </c>
+      <c r="J13">
+        <v>1.7919884666872614</v>
+      </c>
+      <c r="L13">
+        <f>C13*(Variables!L$23/Variables!L$14)</f>
+        <v>9.8678414096916287E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>593</v>
+      </c>
+      <c r="B14">
+        <v>0.35</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:F14" si="8">C4</f>
+        <v>0.15679878540876441</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="8"/>
+        <v>6.6470588235294121</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="8"/>
+        <v>0.16528408426291219</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="8"/>
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="H14" t="s">
+        <v>632</v>
+      </c>
+      <c r="J14">
+        <v>0.38083634706418507</v>
+      </c>
+      <c r="L14">
+        <f>C14*(Variables!L$23/Variables!L$14)</f>
+        <v>4.4403195867968683E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>594</v>
+      </c>
+      <c r="B15">
+        <v>0.35</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:F15" si="9">C11</f>
+        <v>0.19196328081035452</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="9"/>
+        <v>6.6470588235294121</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="9"/>
+        <v>0.13960965877116693</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="9"/>
+        <v>0.32944009850789513</v>
+      </c>
+      <c r="H15" t="s">
+        <v>633</v>
+      </c>
+      <c r="J15">
+        <v>0.32944009850789513</v>
+      </c>
+      <c r="L15">
+        <f>C15*(Variables!L$23/Variables!L$14)</f>
+        <v>5.4361283061339333E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>595</v>
+      </c>
+      <c r="B16">
+        <v>0.35</v>
+      </c>
+      <c r="C16">
+        <f>(Variables!L18/Variables!L23)*(stoe!B7/(6-((21/2)*stoe!B7)))</f>
+        <v>0.59266453382084072</v>
+      </c>
+      <c r="D16">
+        <f>(Variables!L18/Variables!L26)</f>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E16">
+        <f>(Variables!L18/Variables!L24)*(stoe!B7/(6-(10*stoe!B7)))</f>
+        <v>0.41509282970550565</v>
+      </c>
+      <c r="F16">
+        <f>(Variables!L18/Variables!L22)*(stoe!B7/(6-(7*stoe!B7)))</f>
+        <v>0.83045148895292964</v>
+      </c>
+      <c r="H16" t="s">
+        <v>634</v>
+      </c>
+      <c r="J16">
+        <v>0.83045148895292964</v>
+      </c>
+      <c r="L16">
+        <f>C16*(Variables!L$23/Variables!L$18)</f>
+        <v>7.6782449725776941E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B17">
+        <v>0.35</v>
+      </c>
+      <c r="C17">
+        <f>(Variables!L18/Variables!L23)*(stoe!B8/((33/2)-((21/2)*stoe!B8)))</f>
+        <v>0.34183471727955711</v>
+      </c>
+      <c r="D17">
+        <f>(Variables!L18/Variables!L26)*(stoe!B8/(4-stoe!B8))</f>
+        <v>2.0698699461283123</v>
+      </c>
+      <c r="E17">
+        <f>(Variables!L18/Variables!L24)*(stoe!B8/(16-(10*stoe!B8)))</f>
+        <v>0.25426470588235289</v>
+      </c>
+      <c r="F17">
+        <f>(Variables!L18/Variables!L22)*(stoe!B8/(6-(7*stoe!B8)))</f>
+        <v>2.7284986729789824</v>
+      </c>
+      <c r="H17" t="s">
+        <v>610</v>
+      </c>
+      <c r="J17">
+        <v>2.7284986729789824</v>
+      </c>
+      <c r="L17">
+        <f>C17*(Variables!L$23/Variables!L$18)</f>
+        <v>4.4286279161724E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>597</v>
+      </c>
+      <c r="B18">
+        <v>0.35</v>
+      </c>
+      <c r="C18">
+        <f>(Variables!L18/Variables!L23)*(stoe!B9/((139/4)-((21/2)*stoe!B9)))</f>
+        <v>0.14872079850398687</v>
+      </c>
+      <c r="D18">
+        <f>(Variables!L18/Variables!L26)</f>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E18">
+        <f>(Variables!L18/Variables!L24)*(stoe!B9/(25-(10*stoe!B9)))</f>
+        <v>0.16088252564187555</v>
+      </c>
+      <c r="F18">
+        <f>(Variables!L18/Variables!L22)*(stoe!B9/((45/2)-(7*stoe!B9)))</f>
+        <v>0.41080205601442249</v>
+      </c>
+      <c r="H18" t="s">
+        <v>612</v>
+      </c>
+      <c r="J18">
+        <v>0.41080205601442249</v>
+      </c>
+      <c r="L18">
+        <f>C18*(Variables!L$23/Variables!L$18)</f>
+        <v>1.9267471870961863E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>598</v>
+      </c>
+      <c r="B19">
+        <v>0.35</v>
+      </c>
+      <c r="C19">
+        <f>(Variables!L19/Variables!L23)*(stoe!B10/(10-((21/2)*stoe!B10)))</f>
+        <v>0.18993587130957534</v>
+      </c>
+      <c r="D19">
+        <f>Variables!L19/Variables!L26</f>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E19">
+        <f>(Variables!L19/Variables!L24)*(stoe!B10/(10-(10*stoe!B10)))</f>
+        <v>0.13645628402800014</v>
+      </c>
+      <c r="F19">
+        <f>(Variables!L19/Variables!L22)*(stoe!B10/(9-(7*stoe!B10)))</f>
+        <v>0.35162784939961444</v>
+      </c>
+      <c r="H19" t="s">
+        <v>614</v>
+      </c>
+      <c r="J19">
+        <v>0.35162784939961444</v>
+      </c>
+      <c r="L19">
+        <f>C19*(Variables!L$23/Variables!L$18)</f>
+        <v>2.4607076444965226E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>599</v>
+      </c>
+      <c r="B20">
+        <v>0.35</v>
+      </c>
+      <c r="C20">
+        <f>(Variables!L19/Variables!L23)*(stoe!B11/((49/2)-((21/2)*stoe!B11)))</f>
+        <v>0.21008868149029522</v>
+      </c>
+      <c r="D20">
+        <f>(Variables!L19/Variables!L26)</f>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E20">
+        <f>(Variables!L19/Variables!L24)*(stoe!B11/(20-(10*stoe!B11)))</f>
+        <v>0.19653096971353326</v>
+      </c>
+      <c r="F20">
+        <f>(Variables!L19/Variables!L22)*(stoe!B11/(15-(7*stoe!B11)))</f>
+        <v>0.6259362128927346</v>
+      </c>
+      <c r="H20" t="s">
+        <v>616</v>
+      </c>
+      <c r="J20">
+        <v>0.6259362128927346</v>
+      </c>
+      <c r="L20">
+        <f>C20*(Variables!L$23/Variables!L$18)</f>
+        <v>2.7217966832750799E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>600</v>
+      </c>
+      <c r="B21">
+        <v>0.35</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:F21" si="10">C16</f>
+        <v>0.59266453382084072</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="10"/>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="10"/>
+        <v>0.41509282970550565</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="10"/>
+        <v>0.83045148895292964</v>
+      </c>
+      <c r="H21" t="s">
+        <v>617</v>
+      </c>
+      <c r="J21">
+        <v>0.83045148895292964</v>
+      </c>
+      <c r="L21">
+        <f>C21*(Variables!L$23/Variables!L$18)</f>
+        <v>7.6782449725776941E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>601</v>
+      </c>
+      <c r="B22">
+        <v>0.35</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:F22" si="11">C17</f>
+        <v>0.34183471727955711</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="11"/>
+        <v>2.0698699461283123</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="11"/>
+        <v>0.25426470588235289</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="11"/>
+        <v>2.7284986729789824</v>
+      </c>
+      <c r="H22" t="s">
+        <v>611</v>
+      </c>
+      <c r="J22">
+        <v>2.7284986729789824</v>
+      </c>
+      <c r="L22">
+        <f>C22*(Variables!L$23/Variables!L$18)</f>
+        <v>4.4286279161724E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>602</v>
+      </c>
+      <c r="B23">
+        <v>0.35</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:F23" si="12">C18</f>
+        <v>0.14872079850398687</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="12"/>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="12"/>
+        <v>0.16088252564187555</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="12"/>
+        <v>0.41080205601442249</v>
+      </c>
+      <c r="H23" t="s">
+        <v>613</v>
+      </c>
+      <c r="J23">
+        <v>0.41080205601442249</v>
+      </c>
+      <c r="L23">
+        <f>C23*(Variables!L$23/Variables!L$18)</f>
+        <v>1.9267471870961863E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>603</v>
+      </c>
+      <c r="B24">
+        <v>0.35</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:F24" si="13">C19</f>
+        <v>0.18993587130957534</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="13"/>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="13"/>
+        <v>0.13645628402800014</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="13"/>
+        <v>0.35162784939961444</v>
+      </c>
+      <c r="H24" t="s">
+        <v>615</v>
+      </c>
+      <c r="J24">
+        <v>0.35162784939961444</v>
+      </c>
+      <c r="L24">
+        <f>C24*(Variables!L$23/Variables!L$18)</f>
+        <v>2.4607076444965226E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>604</v>
+      </c>
+      <c r="B25">
+        <v>0.35</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:F25" si="14">C20</f>
+        <v>0.21008868149029522</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="14"/>
+        <v>14.529411764705882</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="14"/>
+        <v>0.19653096971353326</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="14"/>
+        <v>0.6259362128927346</v>
+      </c>
+      <c r="H25" t="s">
+        <v>618</v>
+      </c>
+      <c r="J25">
+        <v>0.6259362128927346</v>
+      </c>
+      <c r="L25">
+        <f>C25*(Variables!L$23/Variables!L$18)</f>
+        <v>2.7217966832750799E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>635</v>
+      </c>
+      <c r="B26">
+        <v>0.13</v>
+      </c>
+      <c r="C26">
+        <f>(stoe!B15/stoe!B13)*(Variables!L21/Variables!L23)</f>
+        <v>4.0522540983606553E-2</v>
+      </c>
+      <c r="F26">
+        <f>(stoe!B15/stoe!B16)*(Variables!L20/Variables!L22)</f>
+        <v>0.1266410502721742</v>
+      </c>
+      <c r="G26">
+        <f>(stoe!B15/stoe!B17)*(Variables!L20/Variables!L25)</f>
+        <v>3.9055299539170509E-2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>651</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDDFCB-2B9F-4872-A820-97635CABD872}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51847,793 +52811,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD039EB6-CAC1-4780-9B81-62B23D513731}">
-  <dimension ref="A1:J26"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C1" t="s">
-        <v>606</v>
-      </c>
-      <c r="D1" t="s">
-        <v>607</v>
-      </c>
-      <c r="E1" t="s">
-        <v>608</v>
-      </c>
-      <c r="F1" t="s">
-        <v>609</v>
-      </c>
-      <c r="G1" t="s">
-        <v>637</v>
-      </c>
-      <c r="H1" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>581</v>
-      </c>
-      <c r="B2">
-        <v>0.35</v>
-      </c>
-      <c r="C2">
-        <f>(Variables!L14/Variables!L23)*(stoe!B3/(6-(5*stoe!B3)))</f>
-        <v>0.61286157024793375</v>
-      </c>
-      <c r="D2">
-        <f>(Variables!M14/Variables!L26)</f>
-        <v>0.70588235294117652</v>
-      </c>
-      <c r="E2">
-        <f>(stoe!B3/(6-5*(stoe!B3)))*(Variables!L14/Variables!L24)</f>
-        <v>0.44571750563486096</v>
-      </c>
-      <c r="F2">
-        <f>(Variables!L14/Variables!L22)*(stoe!B3/(6-(2*stoe!B3)))</f>
-        <v>0.71648550724637672</v>
-      </c>
-      <c r="H2" t="s">
-        <v>620</v>
-      </c>
-      <c r="J2">
-        <v>0.71648550724637672</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>582</v>
-      </c>
-      <c r="B3">
-        <v>0.35</v>
-      </c>
-      <c r="C3">
-        <f>(Variables!L15/Variables!L23)*(stoe!B4/((33/2)-(5*stoe!B4)))</f>
-        <v>0.34845814977973566</v>
-      </c>
-      <c r="D3">
-        <f>(Variables!L14/Variables!L26)*(stoe!B4/(4-stoe!B4))</f>
-        <v>2.4906254472591955</v>
-      </c>
-      <c r="E3">
-        <f>(Variables!L14/Variables!L24)*(stoe!B4/(15-(5*stoe!B4)))</f>
-        <v>0.29323447636700645</v>
-      </c>
-      <c r="F3">
-        <f>(Variables!L14/Variables!L22)*(stoe!B4/(6-(2*stoe!B4)))</f>
-        <v>1.7919884666872614</v>
-      </c>
-      <c r="H3" t="s">
-        <v>621</v>
-      </c>
-      <c r="J3">
-        <v>1.7919884666872614</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>583</v>
-      </c>
-      <c r="B4">
-        <v>0.35</v>
-      </c>
-      <c r="C4">
-        <f>(Variables!L14/Variables!L23)*(stoe!B5/((134/4)-(5*stoe!B5)))</f>
-        <v>0.15679878540876441</v>
-      </c>
-      <c r="D4">
-        <f>(Variables!L14/Variables!L26)</f>
-        <v>6.6470588235294121</v>
-      </c>
-      <c r="E4">
-        <f>(Variables!L14/Variables!L24)*(stoe!B5/(25-(5*stoe!B5)))</f>
-        <v>0.16528408426291219</v>
-      </c>
-      <c r="F4">
-        <f>(Variables!L14/Variables!L22)*(stoe!B5/((45/2)-(2*stoe!B5)))</f>
-        <v>0.38083634706418507</v>
-      </c>
-      <c r="H4" t="s">
-        <v>622</v>
-      </c>
-      <c r="J4">
-        <v>0.38083634706418507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>584</v>
-      </c>
-      <c r="B5">
-        <v>0.35</v>
-      </c>
-      <c r="C5">
-        <f>C2</f>
-        <v>0.61286157024793375</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:F5" si="0">D2</f>
-        <v>0.70588235294117652</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0.44571750563486096</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0.71648550724637672</v>
-      </c>
-      <c r="H5" t="s">
-        <v>623</v>
-      </c>
-      <c r="J5">
-        <v>0.71648550724637672</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>585</v>
-      </c>
-      <c r="B6">
-        <v>0.35</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ref="C6:F6" si="1">C3</f>
-        <v>0.34845814977973566</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>2.4906254472591955</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0.29323447636700645</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>1.7919884666872614</v>
-      </c>
-      <c r="H6" t="s">
-        <v>624</v>
-      </c>
-      <c r="J6">
-        <v>1.7919884666872614</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>586</v>
-      </c>
-      <c r="B7">
-        <v>0.35</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ref="C7:F7" si="2">C4</f>
-        <v>0.15679878540876441</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="2"/>
-        <v>6.6470588235294121</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>0.16528408426291219</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>0.38083634706418507</v>
-      </c>
-      <c r="H7" t="s">
-        <v>625</v>
-      </c>
-      <c r="J7">
-        <v>0.38083634706418507</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>587</v>
-      </c>
-      <c r="B8">
-        <v>0.35</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:F8" si="3">C2</f>
-        <v>0.61286157024793375</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="3"/>
-        <v>0.70588235294117652</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="3"/>
-        <v>0.44571750563486096</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>0.71648550724637672</v>
-      </c>
-      <c r="H8" t="s">
-        <v>626</v>
-      </c>
-      <c r="J8">
-        <v>0.71648550724637672</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>588</v>
-      </c>
-      <c r="B9">
-        <v>0.35</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9:F9" si="4">C3</f>
-        <v>0.34845814977973566</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="4"/>
-        <v>2.4906254472591955</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="4"/>
-        <v>0.29323447636700645</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="4"/>
-        <v>1.7919884666872614</v>
-      </c>
-      <c r="H9" t="s">
-        <v>627</v>
-      </c>
-      <c r="J9">
-        <v>1.7919884666872614</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>589</v>
-      </c>
-      <c r="B10">
-        <v>0.35</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ref="C10:F10" si="5">C4</f>
-        <v>0.15679878540876441</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="5"/>
-        <v>6.6470588235294121</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="5"/>
-        <v>0.16528408426291219</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="5"/>
-        <v>0.38083634706418507</v>
-      </c>
-      <c r="H10" t="s">
-        <v>628</v>
-      </c>
-      <c r="J10">
-        <v>0.38083634706418507</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>590</v>
-      </c>
-      <c r="B11">
-        <v>0.35</v>
-      </c>
-      <c r="C11">
-        <f>(Variables!L16/Variables!L23)*(stoe!B6/(10-(5*stoe!B6)))</f>
-        <v>0.19196328081035452</v>
-      </c>
-      <c r="D11">
-        <f>(Variables!L16/Variables!L26)</f>
-        <v>6.6470588235294121</v>
-      </c>
-      <c r="E11">
-        <f>(Variables!L16/Variables!L24)*(stoe!B6/(10-(5*stoe!B6)))</f>
-        <v>0.13960965877116693</v>
-      </c>
-      <c r="F11">
-        <f>(Variables!L16/Variables!L22)*(stoe!B6/(9-(2*stoe!B6)))</f>
-        <v>0.32944009850789513</v>
-      </c>
-      <c r="H11" t="s">
-        <v>629</v>
-      </c>
-      <c r="J11">
-        <v>0.32944009850789513</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>591</v>
-      </c>
-      <c r="B12">
-        <v>0.35</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:F12" si="6">C2</f>
-        <v>0.61286157024793375</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="6"/>
-        <v>0.70588235294117652</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="6"/>
-        <v>0.44571750563486096</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="6"/>
-        <v>0.71648550724637672</v>
-      </c>
-      <c r="H12" t="s">
-        <v>630</v>
-      </c>
-      <c r="J12">
-        <v>0.71648550724637672</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>592</v>
-      </c>
-      <c r="B13">
-        <v>0.35</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ref="C13:F13" si="7">C3</f>
-        <v>0.34845814977973566</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="7"/>
-        <v>2.4906254472591955</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="7"/>
-        <v>0.29323447636700645</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="7"/>
-        <v>1.7919884666872614</v>
-      </c>
-      <c r="H13" t="s">
-        <v>631</v>
-      </c>
-      <c r="J13">
-        <v>1.7919884666872614</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>593</v>
-      </c>
-      <c r="B14">
-        <v>0.35</v>
-      </c>
-      <c r="C14">
-        <f t="shared" ref="C14:F14" si="8">C4</f>
-        <v>0.15679878540876441</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="8"/>
-        <v>6.6470588235294121</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="8"/>
-        <v>0.16528408426291219</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="8"/>
-        <v>0.38083634706418507</v>
-      </c>
-      <c r="H14" t="s">
-        <v>632</v>
-      </c>
-      <c r="J14">
-        <v>0.38083634706418507</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>594</v>
-      </c>
-      <c r="B15">
-        <v>0.35</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:F15" si="9">C11</f>
-        <v>0.19196328081035452</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="9"/>
-        <v>6.6470588235294121</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="9"/>
-        <v>0.13960965877116693</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="9"/>
-        <v>0.32944009850789513</v>
-      </c>
-      <c r="H15" t="s">
-        <v>633</v>
-      </c>
-      <c r="J15">
-        <v>0.32944009850789513</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>595</v>
-      </c>
-      <c r="B16">
-        <v>0.35</v>
-      </c>
-      <c r="C16">
-        <f>(Variables!L18/Variables!L23)*(stoe!B7/(6-((21/2)*stoe!B7)))</f>
-        <v>0.59266453382084072</v>
-      </c>
-      <c r="D16">
-        <f>(Variables!L18/Variables!L26)</f>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E16">
-        <f>(Variables!L18/Variables!L24)*(stoe!B7/(6-(10*stoe!B7)))</f>
-        <v>0.41509282970550565</v>
-      </c>
-      <c r="F16">
-        <f>(Variables!L18/Variables!L22)*(stoe!B7/(6-(7*stoe!B7)))</f>
-        <v>0.83045148895292964</v>
-      </c>
-      <c r="H16" t="s">
-        <v>634</v>
-      </c>
-      <c r="J16">
-        <v>0.83045148895292964</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>596</v>
-      </c>
-      <c r="B17">
-        <v>0.35</v>
-      </c>
-      <c r="C17">
-        <f>(Variables!L18/Variables!L23)*(stoe!B8/((33/2)-((21/2)*stoe!B8)))</f>
-        <v>0.34183471727955711</v>
-      </c>
-      <c r="D17">
-        <f>(Variables!L18/Variables!L26)*(stoe!B8/(4-stoe!B8))</f>
-        <v>2.0698699461283123</v>
-      </c>
-      <c r="E17">
-        <f>(Variables!L18/Variables!L24)*(stoe!B8/(16-(10*stoe!B8)))</f>
-        <v>0.25426470588235289</v>
-      </c>
-      <c r="F17">
-        <f>(Variables!L18/Variables!L22)*(stoe!B8/(6-(7*stoe!B8)))</f>
-        <v>2.7284986729789824</v>
-      </c>
-      <c r="H17" t="s">
-        <v>610</v>
-      </c>
-      <c r="J17">
-        <v>2.7284986729789824</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>597</v>
-      </c>
-      <c r="B18">
-        <v>0.35</v>
-      </c>
-      <c r="C18">
-        <f>(Variables!L18/Variables!L23)*(stoe!B9/((139/4)-((21/2)*stoe!B9)))</f>
-        <v>0.14872079850398687</v>
-      </c>
-      <c r="D18">
-        <f>(Variables!L18/Variables!L26)</f>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E18">
-        <f>(Variables!L18/Variables!L24)*(stoe!B9/(25-(10*stoe!B9)))</f>
-        <v>0.16088252564187555</v>
-      </c>
-      <c r="F18">
-        <f>(Variables!L18/Variables!L22)*(stoe!B9/((45/2)-(7*stoe!B9)))</f>
-        <v>0.41080205601442249</v>
-      </c>
-      <c r="H18" t="s">
-        <v>612</v>
-      </c>
-      <c r="J18">
-        <v>0.41080205601442249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>598</v>
-      </c>
-      <c r="B19">
-        <v>0.35</v>
-      </c>
-      <c r="C19">
-        <f>(Variables!L19/Variables!L23)*(stoe!B10/(10-((21/2)*stoe!B10)))</f>
-        <v>0.18993587130957534</v>
-      </c>
-      <c r="D19">
-        <f>Variables!L19/Variables!L26</f>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E19">
-        <f>(Variables!L19/Variables!L24)*(stoe!B10/(10-(10*stoe!B10)))</f>
-        <v>0.13645628402800014</v>
-      </c>
-      <c r="F19">
-        <f>(Variables!L19/Variables!L22)*(stoe!B10/(9-(7*stoe!B10)))</f>
-        <v>0.35162784939961444</v>
-      </c>
-      <c r="H19" t="s">
-        <v>614</v>
-      </c>
-      <c r="J19">
-        <v>0.35162784939961444</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>599</v>
-      </c>
-      <c r="B20">
-        <v>0.35</v>
-      </c>
-      <c r="C20">
-        <f>(Variables!L19/Variables!L23)*(stoe!B11/((49/2)-((21/2)*stoe!B11)))</f>
-        <v>0.21008868149029522</v>
-      </c>
-      <c r="D20">
-        <f>(Variables!L19/Variables!L26)</f>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E20">
-        <f>(Variables!L19/Variables!L24)*(stoe!B11/(20-(10*stoe!B11)))</f>
-        <v>0.19653096971353326</v>
-      </c>
-      <c r="F20">
-        <f>(Variables!L19/Variables!L22)*(stoe!B11/(15-(7*stoe!B11)))</f>
-        <v>0.6259362128927346</v>
-      </c>
-      <c r="H20" t="s">
-        <v>616</v>
-      </c>
-      <c r="J20">
-        <v>0.6259362128927346</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>600</v>
-      </c>
-      <c r="B21">
-        <v>0.35</v>
-      </c>
-      <c r="C21">
-        <f t="shared" ref="C21:F21" si="10">C16</f>
-        <v>0.59266453382084072</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="10"/>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="10"/>
-        <v>0.41509282970550565</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="10"/>
-        <v>0.83045148895292964</v>
-      </c>
-      <c r="H21" t="s">
-        <v>617</v>
-      </c>
-      <c r="J21">
-        <v>0.83045148895292964</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>601</v>
-      </c>
-      <c r="B22">
-        <v>0.35</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22:F22" si="11">C17</f>
-        <v>0.34183471727955711</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="11"/>
-        <v>2.0698699461283123</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="11"/>
-        <v>0.25426470588235289</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="11"/>
-        <v>2.7284986729789824</v>
-      </c>
-      <c r="H22" t="s">
-        <v>611</v>
-      </c>
-      <c r="J22">
-        <v>2.7284986729789824</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>602</v>
-      </c>
-      <c r="B23">
-        <v>0.35</v>
-      </c>
-      <c r="C23">
-        <f t="shared" ref="C23:F23" si="12">C18</f>
-        <v>0.14872079850398687</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="12"/>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="12"/>
-        <v>0.16088252564187555</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="12"/>
-        <v>0.41080205601442249</v>
-      </c>
-      <c r="H23" t="s">
-        <v>613</v>
-      </c>
-      <c r="J23">
-        <v>0.41080205601442249</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>603</v>
-      </c>
-      <c r="B24">
-        <v>0.35</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:F24" si="13">C19</f>
-        <v>0.18993587130957534</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="13"/>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="13"/>
-        <v>0.13645628402800014</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="13"/>
-        <v>0.35162784939961444</v>
-      </c>
-      <c r="H24" t="s">
-        <v>615</v>
-      </c>
-      <c r="J24">
-        <v>0.35162784939961444</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>604</v>
-      </c>
-      <c r="B25">
-        <v>0.35</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ref="C25:F25" si="14">C20</f>
-        <v>0.21008868149029522</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="14"/>
-        <v>14.529411764705882</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="14"/>
-        <v>0.19653096971353326</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="14"/>
-        <v>0.6259362128927346</v>
-      </c>
-      <c r="H25" t="s">
-        <v>618</v>
-      </c>
-      <c r="J25">
-        <v>0.6259362128927346</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>635</v>
-      </c>
-      <c r="B26">
-        <v>0.13</v>
-      </c>
-      <c r="C26">
-        <f>(stoe!B15/stoe!B13)*(Variables!L21/Variables!L23)</f>
-        <v>4.0522540983606553E-2</v>
-      </c>
-      <c r="F26">
-        <f>(stoe!B15/stoe!B16)*(Variables!L20/Variables!L22)</f>
-        <v>0.1266410502721742</v>
-      </c>
-      <c r="G26">
-        <f>(stoe!B15/stoe!B17)*(Variables!L20/Variables!L25)</f>
-        <v>3.9055299539170509E-2</v>
-      </c>
-      <c r="H26" t="s">
-        <v>636</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E22A85-0A6D-4692-91B9-50CA4D04329A}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53789,7 +53972,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="34" t="s">
         <v>418</v>
       </c>
@@ -54115,14 +54298,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CD580C-396B-4BB3-AD93-6F2493BB33D0}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="5" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="6" width="13.1796875" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
ajout fichier pour validation du modèle
</commit_message>
<xml_diff>
--- a/Data Komilis FWGW.xlsx
+++ b/Data Komilis FWGW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hravoaha\Desktop\Thèse\composting code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD54FE8-57C8-4AA0-BE23-673E892880A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AEC87A-D751-4DD8-8821-9B43EE72C1EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="6" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{14B8D0C9-091E-43B5-9C59-8A05020574F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Composition of waste" sheetId="4" r:id="rId1"/>
@@ -2667,9 +2667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A43F10C-4AB5-4A1F-A346-6667884FAA0F}">
   <dimension ref="A1:CE113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A96" sqref="A96:XFD96"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25972,8 +25972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DF1B96-6F36-403A-A03F-B41BA123E54D}">
   <dimension ref="A1:CD106"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J96" sqref="J96"/>
+    <sheetView topLeftCell="B88" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G100" sqref="G99:G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -50462,8 +50462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13E0657-BE6C-45BC-B891-D54361BD0D37}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51257,7 +51257,7 @@
         <v>1</v>
       </c>
       <c r="L18">
-        <f t="shared" si="0"/>
+        <f>($F18*12)+($G18*1)+($H18*16)+($I18*14)</f>
         <v>247</v>
       </c>
       <c r="M18">
@@ -54298,7 +54298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CD580C-396B-4BB3-AD93-6F2493BB33D0}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>